<commit_message>
added JUnit test cases
added JUnit test cases and test message flow files
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -381,15 +381,6 @@
     <t>The try terminal (output) for '" + msgFlowNode.getName() + "' (type: " + msgFlowNode.getType() + ") is not connected.</t>
   </si>
   <si>
-    <t>TimeoutNotificationFailureTerminal</t>
-  </si>
-  <si>
-    <t>TimeoutNotificationOutTerminal</t>
-  </si>
-  <si>
-    <t>TimeoutNotificationCatchTerminal</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
@@ -523,6 +514,15 @@
   </si>
   <si>
     <t>Reset should be enabled in order to get the message tree parsed again using the given message format.</t>
+  </si>
+  <si>
+    <t>TimeoutNotificationNodeFailureTerminal</t>
+  </si>
+  <si>
+    <t>TimeoutNotificationNodeOutTerminal</t>
+  </si>
+  <si>
+    <t>TimeoutNotificationNodeCatchTerminal</t>
   </si>
 </sst>
 </file>
@@ -895,13 +895,13 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -917,13 +917,13 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
         <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -934,13 +934,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
         <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
         <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -968,13 +968,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
         <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -985,13 +985,13 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
         <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,13 +1007,13 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E9" t="s">
         <v>101</v>
       </c>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,13 +1024,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E10" t="s">
         <v>97</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,13 +1041,13 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E11" t="s">
         <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1063,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
         <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1080,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1097,13 +1097,13 @@
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E15" t="s">
         <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1114,13 +1114,13 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1131,13 +1131,13 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
         <v>103</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1148,13 +1148,13 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
         <v>104</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1165,13 +1165,13 @@
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E19" t="s">
         <v>105</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,13 +1182,13 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
         <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1199,13 +1199,13 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E21" t="s">
         <v>107</v>
       </c>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,13 +1216,13 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
         <v>108</v>
       </c>
       <c r="F22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1238,30 +1238,30 @@
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E24" t="s">
         <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E25" t="s">
         <v>109</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,13 +1272,13 @@
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
         <v>97</v>
       </c>
       <c r="F26" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,30 +1289,30 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E27" t="s">
         <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E28" t="s">
         <v>102</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1323,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E29" t="s">
         <v>106</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1345,13 +1345,13 @@
         <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E31" t="s">
         <v>97</v>
       </c>
       <c r="F31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,13 +1362,13 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
       </c>
       <c r="F32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1379,13 +1379,13 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E33" t="s">
         <v>111</v>
       </c>
       <c r="F33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1396,13 +1396,13 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s">
         <v>100</v>
       </c>
       <c r="F34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,13 +1413,13 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E35" t="s">
         <v>103</v>
       </c>
       <c r="F35" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1430,13 +1430,13 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E36" t="s">
         <v>104</v>
       </c>
       <c r="F36" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,13 +1447,13 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E37" t="s">
         <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1464,13 +1464,13 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E38" t="s">
         <v>106</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,13 +1481,13 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E39" t="s">
         <v>107</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1498,13 +1498,13 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
         <v>108</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1520,13 +1520,13 @@
         <v>2</v>
       </c>
       <c r="D42" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E42" t="s">
         <v>112</v>
       </c>
       <c r="F42" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,13 +1537,13 @@
         <v>2</v>
       </c>
       <c r="D43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E43" t="s">
         <v>113</v>
       </c>
       <c r="F43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,13 +1554,13 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
         <v>101</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1571,13 +1571,13 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E45" t="s">
         <v>97</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1588,13 +1588,13 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E46" t="s">
         <v>98</v>
       </c>
       <c r="F46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1605,13 +1605,13 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E47" t="s">
         <v>114</v>
       </c>
       <c r="F47" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1622,13 +1622,13 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E48" t="s">
         <v>103</v>
       </c>
       <c r="F48" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1639,13 +1639,13 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E49" t="s">
         <v>104</v>
       </c>
       <c r="F49" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1656,13 +1656,13 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E50" t="s">
         <v>105</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1673,13 +1673,13 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E51" t="s">
         <v>106</v>
       </c>
       <c r="F51" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1690,13 +1690,13 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E52" t="s">
         <v>115</v>
       </c>
       <c r="F52" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,13 +1707,13 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E53" t="s">
         <v>116</v>
       </c>
       <c r="F53" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1729,13 +1729,13 @@
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
         <v>97</v>
       </c>
       <c r="F55" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1746,13 +1746,13 @@
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E56" t="s">
         <v>98</v>
       </c>
       <c r="F56" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1763,13 +1763,13 @@
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E57" t="s">
         <v>100</v>
       </c>
       <c r="F57" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1780,13 +1780,13 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E58" t="s">
         <v>103</v>
       </c>
       <c r="F58" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E59" t="s">
         <v>104</v>
       </c>
       <c r="F59" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1814,13 +1814,13 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E60" t="s">
         <v>105</v>
       </c>
       <c r="F60" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,13 +1831,13 @@
         <v>2</v>
       </c>
       <c r="D61" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E61" t="s">
         <v>106</v>
       </c>
       <c r="F61" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1848,13 +1848,13 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E62" t="s">
         <v>107</v>
       </c>
       <c r="F62" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1865,13 +1865,13 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E63" t="s">
         <v>108</v>
       </c>
       <c r="F63" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,13 +1887,13 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E65" t="s">
         <v>101</v>
       </c>
       <c r="F65" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1904,13 +1904,13 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E66" t="s">
         <v>97</v>
       </c>
       <c r="F66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1921,13 +1921,13 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E67" t="s">
         <v>98</v>
       </c>
       <c r="F67" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1938,13 +1938,13 @@
         <v>2</v>
       </c>
       <c r="D68" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E68" t="s">
         <v>106</v>
       </c>
       <c r="F68" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1954,104 +1954,104 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C70" t="s">
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F70" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F71" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F72" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F73" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F74" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F75" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2067,13 +2067,13 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E77" t="s">
         <v>97</v>
       </c>
       <c r="F77" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,13 +2084,13 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E78" t="s">
         <v>98</v>
       </c>
       <c r="F78" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2101,13 +2101,13 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E79" t="s">
         <v>111</v>
       </c>
       <c r="F79" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,13 +2118,13 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E80" t="s">
         <v>100</v>
       </c>
       <c r="F80" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2135,13 +2135,13 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E81" t="s">
         <v>103</v>
       </c>
       <c r="F81" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2152,13 +2152,13 @@
         <v>2</v>
       </c>
       <c r="D82" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E82" t="s">
         <v>106</v>
       </c>
       <c r="F82" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2174,13 +2174,13 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E84" t="s">
         <v>101</v>
       </c>
       <c r="F84" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,13 +2191,13 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E85" t="s">
         <v>98</v>
       </c>
       <c r="F85" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,13 +2208,13 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
         <v>97</v>
       </c>
       <c r="F86" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2225,13 +2225,13 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E87" t="s">
         <v>117</v>
       </c>
       <c r="F87" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2242,13 +2242,13 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
         <v>103</v>
       </c>
       <c r="F88" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2259,13 +2259,13 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E89" t="s">
         <v>106</v>
       </c>
       <c r="F89" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,13 +2281,13 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E91" t="s">
         <v>101</v>
       </c>
       <c r="F91" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2298,13 +2298,13 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E92" t="s">
         <v>97</v>
       </c>
       <c r="F92" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,13 +2315,13 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E93" t="s">
         <v>98</v>
       </c>
       <c r="F93" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2331,53 +2331,53 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E95" t="s">
         <v>97</v>
       </c>
       <c r="F95" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E96" t="s">
         <v>98</v>
       </c>
       <c r="F96" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="C97" t="s">
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E97" t="s">
         <v>100</v>
       </c>
       <c r="F97" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2393,13 +2393,13 @@
         <v>3</v>
       </c>
       <c r="D99" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E99" t="s">
         <v>118</v>
       </c>
       <c r="F99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E100" t="s">
         <v>101</v>
       </c>
       <c r="F100" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2427,13 +2427,13 @@
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E101" t="s">
         <v>119</v>
       </c>
       <c r="F101" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2444,13 +2444,13 @@
         <v>3</v>
       </c>
       <c r="D102" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E102" t="s">
         <v>100</v>
       </c>
       <c r="F102" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2482,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2490,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2498,7 +2498,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added monitoring event rules
added monitoring event rules and JUnit test cases
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="184">
   <si>
     <t>severity</t>
   </si>
@@ -523,13 +523,61 @@
   </si>
   <si>
     <t>TimeoutNotificationNodeCatchTerminal</t>
+  </si>
+  <si>
+    <t>ComputeNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>There are no monitoring events defined or the existing events are disabled for '" + msgFlowNode.getName() + "' (type: " + msgFlowNode.getType() + ") (see Properties).</t>
+  </si>
+  <si>
+    <t>Events are used to support transaction monitoring, transaction auditing and business process monitoring. Enable monitoring events if you need that support.</t>
+  </si>
+  <si>
+    <t>CollectorNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>FileInputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>FileOutputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>HttpInputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>HttpRequestNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>MQInputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>MQOutputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>ResetContentDescriptorNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>SoapInputNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>SoapRequestNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>TimeoutControlNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>TimeoutNotificationNodeMonitoringEvents</t>
+  </si>
+  <si>
+    <t>TryCatchNodeMonitoringEvents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +589,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,10 +620,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -871,7 +926,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -881,7 +936,7 @@
     <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.7109375" customWidth="1"/>
-    <col min="6" max="6" width="135.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="142.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,30 +1050,27 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1027,71 +1079,71 @@
         <v>121</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" t="s">
         <v>98</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>121</v>
       </c>
-      <c r="E13" t="s">
-        <v>97</v>
-      </c>
-      <c r="F13" t="s">
-        <v>125</v>
+      <c r="E13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" t="s">
-        <v>127</v>
+      <c r="A14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1100,15 +1152,15 @@
         <v>121</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
@@ -1117,15 +1169,15 @@
         <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
@@ -1134,15 +1186,15 @@
         <v>121</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -1151,15 +1203,15 @@
         <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
@@ -1168,49 +1220,49 @@
         <v>121</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
         <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
         <v>121</v>
       </c>
       <c r="E21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
@@ -1219,71 +1271,68 @@
         <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
         <v>121</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F24" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>135</v>
+      <c r="B25" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>121</v>
       </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" t="s">
-        <v>144</v>
+      <c r="E25" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" t="s">
-        <v>125</v>
+      <c r="A26" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
@@ -1292,15 +1341,15 @@
         <v>121</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
@@ -1309,37 +1358,49 @@
         <v>121</v>
       </c>
       <c r="E28" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F28" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
         <v>121</v>
       </c>
       <c r="E29" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>32</v>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
@@ -1348,66 +1409,51 @@
         <v>121</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>110</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
         <v>121</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>34</v>
+      <c r="B33" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
         <v>121</v>
       </c>
-      <c r="E33" t="s">
-        <v>111</v>
-      </c>
-      <c r="F33" t="s">
-        <v>143</v>
+      <c r="E33" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" t="s">
-        <v>126</v>
+      <c r="A34" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>3</v>
@@ -1416,15 +1462,15 @@
         <v>121</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F35" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
@@ -1433,15 +1479,15 @@
         <v>121</v>
       </c>
       <c r="E36" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
         <v>3</v>
@@ -1450,71 +1496,83 @@
         <v>121</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
         <v>121</v>
       </c>
       <c r="E38" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" t="s">
         <v>121</v>
       </c>
       <c r="E39" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F39" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
         <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F40" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>42</v>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -1523,15 +1581,15 @@
         <v>121</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F42" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -1540,100 +1598,85 @@
         <v>121</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F43" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
         <v>121</v>
       </c>
       <c r="E44" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>46</v>
+      <c r="B45" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
         <v>121</v>
       </c>
-      <c r="E45" t="s">
-        <v>97</v>
-      </c>
-      <c r="F45" t="s">
-        <v>125</v>
+      <c r="E45" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>47</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" t="s">
-        <v>121</v>
-      </c>
-      <c r="E46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" t="s">
-        <v>127</v>
+      <c r="A46" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
         <v>121</v>
       </c>
       <c r="E47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C48" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D48" t="s">
         <v>121</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="F48" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
         <v>3</v>
@@ -1642,15 +1685,15 @@
         <v>121</v>
       </c>
       <c r="E49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F49" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
         <v>3</v>
@@ -1659,71 +1702,83 @@
         <v>121</v>
       </c>
       <c r="E50" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51" t="s">
         <v>121</v>
       </c>
       <c r="E51" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F51" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
         <v>121</v>
       </c>
       <c r="E52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F52" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" t="s">
         <v>121</v>
       </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="F53" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>55</v>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>121</v>
+      </c>
+      <c r="E54" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
         <v>3</v>
@@ -1732,156 +1787,153 @@
         <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F55" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
         <v>121</v>
       </c>
       <c r="E56" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F56" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D57" t="s">
         <v>121</v>
       </c>
       <c r="E57" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="F57" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
         <v>121</v>
       </c>
       <c r="E58" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F58" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>60</v>
+      <c r="B59" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D59" t="s">
         <v>121</v>
       </c>
-      <c r="E59" t="s">
-        <v>104</v>
-      </c>
-      <c r="F59" t="s">
-        <v>139</v>
+      <c r="E59" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" t="s">
-        <v>105</v>
-      </c>
-      <c r="F60" t="s">
-        <v>140</v>
+      <c r="A60" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D61" t="s">
         <v>121</v>
       </c>
       <c r="E61" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F61" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" t="s">
         <v>121</v>
       </c>
       <c r="E62" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F62" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
         <v>121</v>
       </c>
       <c r="E63" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F63" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>65</v>
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" t="s">
+        <v>121</v>
+      </c>
+      <c r="E64" t="s">
+        <v>103</v>
+      </c>
+      <c r="F64" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
@@ -1890,15 +1942,15 @@
         <v>121</v>
       </c>
       <c r="E65" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F65" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
         <v>3</v>
@@ -1907,32 +1959,32 @@
         <v>121</v>
       </c>
       <c r="E66" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F66" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D67" t="s">
         <v>121</v>
       </c>
       <c r="E67" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F67" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
@@ -1941,54 +1993,51 @@
         <v>121</v>
       </c>
       <c r="E68" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F68" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>70</v>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>149</v>
+      <c r="B70" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="C70" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
         <v>121</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F70" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>150</v>
-      </c>
-      <c r="C71" t="s">
-        <v>3</v>
-      </c>
-      <c r="D71" t="s">
-        <v>121</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F71" t="s">
-        <v>132</v>
+      <c r="A71" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
@@ -1996,16 +2045,16 @@
       <c r="D72" t="s">
         <v>121</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>160</v>
+      <c r="E72" t="s">
+        <v>101</v>
       </c>
       <c r="F72" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>152</v>
+        <v>67</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
@@ -2013,16 +2062,16 @@
       <c r="D73" t="s">
         <v>121</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>157</v>
+      <c r="E73" t="s">
+        <v>97</v>
       </c>
       <c r="F73" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>153</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
@@ -2030,55 +2079,52 @@
       <c r="D74" t="s">
         <v>121</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>159</v>
+      <c r="E74" t="s">
+        <v>98</v>
       </c>
       <c r="F74" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>154</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
         <v>121</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>158</v>
+      <c r="E75" t="s">
+        <v>106</v>
       </c>
       <c r="F75" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>71</v>
+      <c r="B76" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>121</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77" t="s">
-        <v>3</v>
-      </c>
-      <c r="D77" t="s">
-        <v>121</v>
-      </c>
-      <c r="E77" t="s">
-        <v>97</v>
-      </c>
-      <c r="F77" t="s">
-        <v>125</v>
+      <c r="A77" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>73</v>
+        <v>149</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
@@ -2086,16 +2132,16 @@
       <c r="D78" t="s">
         <v>121</v>
       </c>
-      <c r="E78" t="s">
-        <v>98</v>
+      <c r="E78" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="F78" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
@@ -2103,16 +2149,16 @@
       <c r="D79" t="s">
         <v>121</v>
       </c>
-      <c r="E79" t="s">
-        <v>111</v>
+      <c r="E79" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="F79" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
@@ -2120,16 +2166,16 @@
       <c r="D80" t="s">
         <v>121</v>
       </c>
-      <c r="E80" t="s">
-        <v>100</v>
+      <c r="E80" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="F80" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="C81" t="s">
         <v>3</v>
@@ -2137,72 +2183,69 @@
       <c r="D81" t="s">
         <v>121</v>
       </c>
-      <c r="E81" t="s">
-        <v>103</v>
+      <c r="E81" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="F81" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>77</v>
+        <v>153</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
         <v>121</v>
       </c>
-      <c r="E82" t="s">
-        <v>106</v>
+      <c r="E82" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="F82" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>78</v>
+      <c r="B83" t="s">
+        <v>154</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>121</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F83" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>79</v>
+      <c r="B84" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D84" t="s">
         <v>121</v>
       </c>
-      <c r="E84" t="s">
-        <v>101</v>
-      </c>
-      <c r="F84" t="s">
-        <v>129</v>
+      <c r="E84" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>80</v>
-      </c>
-      <c r="C85" t="s">
-        <v>3</v>
-      </c>
-      <c r="D85" t="s">
-        <v>121</v>
-      </c>
-      <c r="E85" t="s">
-        <v>98</v>
-      </c>
-      <c r="F85" t="s">
-        <v>127</v>
+      <c r="A85" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
@@ -2219,7 +2262,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C87" t="s">
         <v>3</v>
@@ -2228,15 +2271,15 @@
         <v>121</v>
       </c>
       <c r="E87" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="F87" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
@@ -2245,93 +2288,102 @@
         <v>121</v>
       </c>
       <c r="E88" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="F88" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
         <v>121</v>
       </c>
       <c r="E89" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F89" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>85</v>
+      <c r="B90" t="s">
+        <v>76</v>
+      </c>
+      <c r="C90" t="s">
+        <v>3</v>
+      </c>
+      <c r="D90" t="s">
+        <v>121</v>
+      </c>
+      <c r="E90" t="s">
+        <v>103</v>
+      </c>
+      <c r="F90" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D91" t="s">
         <v>121</v>
       </c>
       <c r="E91" t="s">
+        <v>106</v>
+      </c>
+      <c r="F91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>121</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" t="s">
+        <v>121</v>
+      </c>
+      <c r="E94" t="s">
         <v>101</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F94" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>87</v>
-      </c>
-      <c r="C92" t="s">
-        <v>3</v>
-      </c>
-      <c r="D92" t="s">
-        <v>121</v>
-      </c>
-      <c r="E92" t="s">
-        <v>97</v>
-      </c>
-      <c r="F92" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" t="s">
-        <v>3</v>
-      </c>
-      <c r="D93" t="s">
-        <v>121</v>
-      </c>
-      <c r="E93" t="s">
-        <v>98</v>
-      </c>
-      <c r="F93" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>165</v>
+        <v>80</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
@@ -2340,15 +2392,15 @@
         <v>121</v>
       </c>
       <c r="E95" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F95" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>166</v>
+        <v>81</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
@@ -2357,15 +2409,15 @@
         <v>121</v>
       </c>
       <c r="E96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F96" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>167</v>
+        <v>82</v>
       </c>
       <c r="C97" t="s">
         <v>3</v>
@@ -2374,95 +2426,298 @@
         <v>121</v>
       </c>
       <c r="E97" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="F97" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>90</v>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+      <c r="C98" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
+        <v>121</v>
+      </c>
+      <c r="E98" t="s">
+        <v>103</v>
+      </c>
+      <c r="F98" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
         <v>121</v>
       </c>
       <c r="E99" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="F99" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>92</v>
+      <c r="B100" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D100" t="s">
         <v>121</v>
       </c>
-      <c r="E100" t="s">
-        <v>101</v>
-      </c>
-      <c r="F100" t="s">
-        <v>129</v>
+      <c r="E100" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>93</v>
-      </c>
-      <c r="C101" t="s">
-        <v>3</v>
-      </c>
-      <c r="D101" t="s">
-        <v>121</v>
-      </c>
-      <c r="E101" t="s">
-        <v>119</v>
-      </c>
-      <c r="F101" t="s">
-        <v>136</v>
+      <c r="A101" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
+        <v>86</v>
+      </c>
+      <c r="C102" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" t="s">
+        <v>101</v>
+      </c>
+      <c r="F102" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>87</v>
+      </c>
+      <c r="C103" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>121</v>
+      </c>
+      <c r="E103" t="s">
+        <v>97</v>
+      </c>
+      <c r="F103" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>88</v>
+      </c>
+      <c r="C104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" t="s">
+        <v>121</v>
+      </c>
+      <c r="E104" t="s">
+        <v>98</v>
+      </c>
+      <c r="F104" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C105" t="s">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>121</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>165</v>
+      </c>
+      <c r="C107" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>121</v>
+      </c>
+      <c r="E107" t="s">
+        <v>97</v>
+      </c>
+      <c r="F107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>166</v>
+      </c>
+      <c r="C108" t="s">
+        <v>3</v>
+      </c>
+      <c r="D108" t="s">
+        <v>121</v>
+      </c>
+      <c r="E108" t="s">
+        <v>98</v>
+      </c>
+      <c r="F108" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C109" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" t="s">
+        <v>121</v>
+      </c>
+      <c r="E109" t="s">
+        <v>100</v>
+      </c>
+      <c r="F109" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B110" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s">
+        <v>121</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>91</v>
+      </c>
+      <c r="C112" t="s">
+        <v>3</v>
+      </c>
+      <c r="D112" t="s">
+        <v>121</v>
+      </c>
+      <c r="E112" t="s">
+        <v>118</v>
+      </c>
+      <c r="F112" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>92</v>
+      </c>
+      <c r="C113" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" t="s">
+        <v>121</v>
+      </c>
+      <c r="E113" t="s">
+        <v>101</v>
+      </c>
+      <c r="F113" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>93</v>
+      </c>
+      <c r="C114" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
+        <v>121</v>
+      </c>
+      <c r="E114" t="s">
+        <v>119</v>
+      </c>
+      <c r="F114" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>94</v>
       </c>
-      <c r="C102" t="s">
-        <v>3</v>
-      </c>
-      <c r="D102" t="s">
-        <v>121</v>
-      </c>
-      <c r="E102" t="s">
+      <c r="C115" t="s">
+        <v>3</v>
+      </c>
+      <c r="D115" t="s">
+        <v>121</v>
+      </c>
+      <c r="E115" t="s">
         <v>100</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F115" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>121</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C116">
       <formula1>severity</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D116">
       <formula1>tags</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new tags and updated the rule sheet
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19320" windowHeight="6420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="3" r:id="rId2"/>
+    <sheet name="New Rules" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="severity">data!$A$2:$A$5</definedName>
     <definedName name="tags">data!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="314">
   <si>
     <t>severity</t>
   </si>
@@ -880,6 +881,97 @@
   </si>
   <si>
     <t>Compute Node - No active monitoring events found.</t>
+  </si>
+  <si>
+    <t>IMS Request</t>
+  </si>
+  <si>
+    <t>MAJOR</t>
+  </si>
+  <si>
+    <t>Standards</t>
+  </si>
+  <si>
+    <t>Name the IMS Request Node with an incremental number in the end in the order it is created. For e.g.  IMS Request 1 , IMS Request 2 and so on.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Readability </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the short and Long Description for the IMS Request Node to include the transaction name and view number of the transaction being invoked. </t>
+  </si>
+  <si>
+    <t>BLOCKER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pitfall </t>
+  </si>
+  <si>
+    <t>Uncheck the option 'Use connection properties defined on Node' . Instead set Configurable service to 'IMSConnectService'</t>
+  </si>
+  <si>
+    <t>CRITICAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t>Ensure Commit mode is set to 0:COMMIT_THEN_SEND</t>
+  </si>
+  <si>
+    <t>Ensure Message Domain is set to 'BLOB'</t>
+  </si>
+  <si>
+    <t>Always mention flow description inside the message flow.</t>
+  </si>
+  <si>
+    <t>MQ Node</t>
+  </si>
+  <si>
+    <t>Avoid looping connections in the message flow. ( Connecting output terminal of a node to its input terminal)</t>
+  </si>
+  <si>
+    <t>MQ INPUT, MQ OUTPUT, MQ GET: Name them using the underlying queue name for clarity</t>
+  </si>
+  <si>
+    <t>MQ HEADER: Do not use this node until standards on its use have been set and agreed.  Manipulate using ESQL instead.</t>
+  </si>
+  <si>
+    <t>RoutingNode / Filter</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Tech.Debt</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Node Type</t>
+  </si>
+  <si>
+    <t>MINOR</t>
+  </si>
+  <si>
+    <t>Name them using one of the following formats, whichever best conveys the intent of the node:
+Is{Condition}
+Has{Condition}
+Can{Condition}
+TrueIf{Condition}
+FalseIf{Condition}
+Eg: IsOutOfStock
+HasTooManyItems
+CanReserveItem
+TrueIfOutOfStockEqY
+FalseIfOutOfStockEqY</t>
+  </si>
+  <si>
+    <t>General Coding</t>
   </si>
 </sst>
 </file>
@@ -929,14 +1021,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -944,14 +1042,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -989,9 +1090,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1026,7 +1127,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1061,7 +1162,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1237,9 +1338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
@@ -3650,7 +3751,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3696,4 +3797,215 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="138.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2">
+        <v>0.25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3">
+        <v>0.25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4">
+        <v>0.25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B8" t="s">
+        <v>296</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" t="s">
+        <v>311</v>
+      </c>
+      <c r="C9">
+        <v>0.25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>289</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>289</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the rulesheet for all 25 rules
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="19320" windowHeight="6420" activeTab="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="349">
   <si>
     <t>severity</t>
   </si>
@@ -972,6 +972,114 @@
   </si>
   <si>
     <t>General Coding</t>
+  </si>
+  <si>
+    <t>MQ INPUT, MQ OUTPUT, MQ GET : Ensure the transaction mode is set to Automatic to use transactions with persistent messages.</t>
+  </si>
+  <si>
+    <t>MQ REPLY : Ensure the transaction mode is set to Automatic to use transactions with persistent messages.</t>
+  </si>
+  <si>
+    <t>Avoid overusing this node as tree copying is processor heavy.  &lt;-- We don't do this.
+Give them verb-noun names in upper-camel case without spaces so  the underlying module can be named normally.  &lt;-- Only do naming convention</t>
+  </si>
+  <si>
+    <t>Transformation Node (ComputeNode)</t>
+  </si>
+  <si>
+    <t>Webservice Node</t>
+  </si>
+  <si>
+    <t>The SOAP Async node 'fault' terminal should be connected</t>
+  </si>
+  <si>
+    <t>Trace nodes should not be used</t>
+  </si>
+  <si>
+    <t>The message flow does not consistently reply to messages/requests</t>
+  </si>
+  <si>
+    <t>Usually the RouteTo and Label are in the same flow as to make things more readable</t>
+  </si>
+  <si>
+    <t>The filter node may not have its connections connected correctly</t>
+  </si>
+  <si>
+    <t>Label has no associated processing logic attached</t>
+  </si>
+  <si>
+    <t>There is no input connection to this node. The code may not be reachable or functioning</t>
+  </si>
+  <si>
+    <t>Use XMLNSC over XMLNS</t>
+  </si>
+  <si>
+    <t>All Nodes</t>
+  </si>
+  <si>
+    <t>Label Node</t>
+  </si>
+  <si>
+    <t>All input terminals are not connected. Processing may not complete normally</t>
+  </si>
+  <si>
+    <t>Filter Node</t>
+  </si>
+  <si>
+    <t>RouteTo Node</t>
+  </si>
+  <si>
+    <t>MessageFlow</t>
+  </si>
+  <si>
+    <t>Trace Node</t>
+  </si>
+  <si>
+    <t>Soap Async Node</t>
+  </si>
+  <si>
+    <t>Ensure that the "Request timeout" property in the SOAP node is set</t>
+  </si>
+  <si>
+    <t>HttpReply Node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Ignore transport failures" property should be set for HTTPReply Node
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Generate default HTTP headers from reply or response" property should be set for HTTPReply Node
+</t>
+  </si>
+  <si>
+    <t>Correctness</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>Correctness, readability</t>
+  </si>
+  <si>
+    <t>Completeness</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>Bad Practice</t>
   </si>
 </sst>
 </file>
@@ -1021,15 +1129,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1041,9 +1157,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1092,7 +1205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1127,7 +1240,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3801,10 +3914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,43 +3925,43 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="138.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="128" style="6" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>287</v>
       </c>
       <c r="B2" t="s">
         <v>288</v>
       </c>
-      <c r="C2">
-        <v>0.25</v>
+      <c r="C2" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D2" t="s">
         <v>289</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3859,13 +3972,13 @@
       <c r="B3" t="s">
         <v>288</v>
       </c>
-      <c r="C3">
-        <v>0.25</v>
+      <c r="C3" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D3" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>292</v>
       </c>
     </row>
@@ -3876,13 +3989,13 @@
       <c r="B4" t="s">
         <v>293</v>
       </c>
-      <c r="C4">
-        <v>0.25</v>
+      <c r="C4" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D4" t="s">
         <v>294</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>295</v>
       </c>
     </row>
@@ -3893,13 +4006,13 @@
       <c r="B5" t="s">
         <v>296</v>
       </c>
-      <c r="C5">
-        <v>0.25</v>
+      <c r="C5" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D5" t="s">
         <v>297</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>298</v>
       </c>
     </row>
@@ -3910,13 +4023,13 @@
       <c r="B6" t="s">
         <v>288</v>
       </c>
-      <c r="C6">
-        <v>0.5</v>
+      <c r="C6" s="8" t="s">
+        <v>342</v>
       </c>
       <c r="D6" t="s">
         <v>289</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>299</v>
       </c>
     </row>
@@ -3927,13 +4040,13 @@
       <c r="B7" t="s">
         <v>288</v>
       </c>
-      <c r="C7">
-        <v>0.25</v>
+      <c r="C7" t="s">
+        <v>341</v>
       </c>
       <c r="D7" t="s">
         <v>291</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>300</v>
       </c>
     </row>
@@ -3944,13 +4057,13 @@
       <c r="B8" t="s">
         <v>296</v>
       </c>
-      <c r="C8">
-        <v>4</v>
+      <c r="C8" t="s">
+        <v>340</v>
       </c>
       <c r="D8" t="s">
         <v>297</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>302</v>
       </c>
     </row>
@@ -3961,13 +4074,13 @@
       <c r="B9" t="s">
         <v>311</v>
       </c>
-      <c r="C9">
-        <v>0.25</v>
+      <c r="C9" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D9" t="s">
         <v>289</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3978,13 +4091,13 @@
       <c r="B10" t="s">
         <v>288</v>
       </c>
-      <c r="C10">
-        <v>0.25</v>
+      <c r="C10" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D10" t="s">
         <v>289</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3995,17 +4108,273 @@
       <c r="B11" t="s">
         <v>288</v>
       </c>
-      <c r="C11">
-        <v>0.25</v>
+      <c r="C11" s="8" t="s">
+        <v>341</v>
       </c>
       <c r="D11" t="s">
         <v>289</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="6" t="s">
         <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="D18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="B19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" t="s">
+        <v>342</v>
+      </c>
+      <c r="D20" t="s">
+        <v>339</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>327</v>
+      </c>
+      <c r="B21" t="s">
+        <v>288</v>
+      </c>
+      <c r="C21" t="s">
+        <v>342</v>
+      </c>
+      <c r="D21" t="s">
+        <v>345</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B22" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" t="s">
+        <v>339</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>331</v>
+      </c>
+      <c r="B23" t="s">
+        <v>288</v>
+      </c>
+      <c r="C23" t="s">
+        <v>343</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>332</v>
+      </c>
+      <c r="B24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C24" t="s">
+        <v>342</v>
+      </c>
+      <c r="D24" t="s">
+        <v>339</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>333</v>
+      </c>
+      <c r="B25" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25" t="s">
+        <v>346</v>
+      </c>
+      <c r="D25" t="s">
+        <v>289</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>334</v>
+      </c>
+      <c r="B26" t="s">
+        <v>296</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D26" t="s">
+        <v>339</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rule : Timeout Interval for AggregateControl Node should be set to finite value
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="352">
   <si>
     <t>severity</t>
   </si>
@@ -1080,6 +1080,15 @@
   </si>
   <si>
     <t>Bad Practice</t>
+  </si>
+  <si>
+    <t>AggregateControl Node</t>
+  </si>
+  <si>
+    <t>1h 30 min</t>
+  </si>
+  <si>
+    <t>The timeout property should be set to a finite value. Otherwise, message flow execution may never completes in case all replies do not arrive.</t>
   </si>
 </sst>
 </file>
@@ -3914,10 +3923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,7 +3935,7 @@
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="128" style="6" customWidth="1"/>
+    <col min="5" max="5" width="117.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4373,6 +4382,23 @@
         <v>319</v>
       </c>
     </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>349</v>
+      </c>
+      <c r="B27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C27" t="s">
+        <v>350</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Module name should match the name of the compute, database or filter node that uses the module.
Nodes should not share the modules.
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="355">
   <si>
     <t>severity</t>
   </si>
@@ -1089,6 +1089,15 @@
   </si>
   <si>
     <t>The timeout property should be set to a finite value. Otherwise, message flow execution may never completes in case all replies do not arrive.</t>
+  </si>
+  <si>
+    <t>Compute/Database/Filter Node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module name match the name of the compute, database, or filter node that uses the module. </t>
+  </si>
+  <si>
+    <t>Multiple nodes should not refer to the same module. Do not share modules between nodes if needed extract common code into shared functions and procedures</t>
   </si>
 </sst>
 </file>
@@ -3923,15 +3932,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="9" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -3940,7 +3949,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>310</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -3958,7 +3967,7 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B2" t="s">
@@ -3975,7 +3984,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B3" t="s">
@@ -3992,7 +4001,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B4" t="s">
@@ -4009,7 +4018,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B5" t="s">
@@ -4026,7 +4035,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>287</v>
       </c>
       <c r="B6" t="s">
@@ -4043,7 +4052,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>313</v>
       </c>
       <c r="B7" t="s">
@@ -4060,7 +4069,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B8" t="s">
@@ -4077,7 +4086,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B9" t="s">
@@ -4094,7 +4103,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B10" t="s">
@@ -4111,7 +4120,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="9" t="s">
         <v>305</v>
       </c>
       <c r="B11" t="s">
@@ -4128,7 +4137,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -4145,7 +4154,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="9" t="s">
         <v>301</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -4162,7 +4171,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="9" t="s">
         <v>317</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -4179,7 +4188,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="9" t="s">
         <v>336</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -4196,7 +4205,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>336</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -4213,7 +4222,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="9" t="s">
         <v>318</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -4230,7 +4239,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="9" t="s">
         <v>327</v>
       </c>
       <c r="B18" t="s">
@@ -4247,7 +4256,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>327</v>
       </c>
       <c r="B19" t="s">
@@ -4264,7 +4273,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>328</v>
       </c>
       <c r="B20" t="s">
@@ -4281,7 +4290,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>327</v>
       </c>
       <c r="B21" t="s">
@@ -4298,7 +4307,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="9" t="s">
         <v>330</v>
       </c>
       <c r="B22" t="s">
@@ -4315,7 +4324,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="9" t="s">
         <v>331</v>
       </c>
       <c r="B23" t="s">
@@ -4332,7 +4341,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="9" t="s">
         <v>332</v>
       </c>
       <c r="B24" t="s">
@@ -4349,7 +4358,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="9" t="s">
         <v>333</v>
       </c>
       <c r="B25" t="s">
@@ -4366,7 +4375,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="9" t="s">
         <v>334</v>
       </c>
       <c r="B26" t="s">
@@ -4383,7 +4392,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="9" t="s">
         <v>349</v>
       </c>
       <c r="B27" t="s">
@@ -4397,6 +4406,40 @@
       </c>
       <c r="E27" s="9" t="s">
         <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B28" t="s">
+        <v>288</v>
+      </c>
+      <c r="C28" t="s">
+        <v>342</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B29" t="s">
+        <v>288</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D29" t="s">
+        <v>289</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rule: Additional instances are allowed at the input node level.
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="357">
   <si>
     <t>severity</t>
   </si>
@@ -1098,6 +1098,12 @@
   </si>
   <si>
     <t>Multiple nodes should not refer to the same module. Do not share modules between nodes if needed extract common code into shared functions and procedures</t>
+  </si>
+  <si>
+    <t>Input Nodes - MQ/HTTP/SOAP/File</t>
+  </si>
+  <si>
+    <t>Multiple instances of the flow are allowed at the input node</t>
   </si>
 </sst>
 </file>
@@ -3932,11 +3938,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4442,6 +4446,23 @@
         <v>354</v>
       </c>
     </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B30" t="s">
+        <v>288</v>
+      </c>
+      <c r="C30" t="s">
+        <v>346</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rule : Subflow which is not referenced anywhere should be removed.
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="360">
   <si>
     <t>severity</t>
   </si>
@@ -1104,6 +1104,16 @@
   </si>
   <si>
     <t>Multiple instances of the flow are allowed at the input node</t>
+  </si>
+  <si>
+    <t>Subflows</t>
+  </si>
+  <si>
+    <t>Completeness,
+Readability</t>
+  </si>
+  <si>
+    <t>Subflow which is not being referenced should be removed</t>
   </si>
 </sst>
 </file>
@@ -3938,9 +3948,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4463,6 +4475,23 @@
         <v>356</v>
       </c>
     </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" t="s">
+        <v>346</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes in rule severity of unused subflow
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -3951,7 +3951,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4483,7 +4483,7 @@
         <v>288</v>
       </c>
       <c r="C31" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
updated the rules.xlsx sheet for rule keys
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="393">
   <si>
     <t>severity</t>
   </si>
@@ -1114,6 +1114,105 @@
   </si>
   <si>
     <t>Subflow which is not being referenced should be removed</t>
+  </si>
+  <si>
+    <t>SelfConnectingNodes</t>
+  </si>
+  <si>
+    <t>MQNodeNameMatchesQueueName</t>
+  </si>
+  <si>
+    <t>IMSRequestDescription</t>
+  </si>
+  <si>
+    <t>IMSRequestNodeDefinedProperties</t>
+  </si>
+  <si>
+    <t>IMSRequestCommitMode</t>
+  </si>
+  <si>
+    <t>IMSRequestMessageDomain</t>
+  </si>
+  <si>
+    <t>MessageFlowDescription</t>
+  </si>
+  <si>
+    <t>MQHeaderNodeDetection</t>
+  </si>
+  <si>
+    <t>FilterNodeNameCheck</t>
+  </si>
+  <si>
+    <t>IMSRequestNodeName</t>
+  </si>
+  <si>
+    <t>MQNodeTxnMode</t>
+  </si>
+  <si>
+    <t>HttpReplyGenerateDefaultHttpHeadersCheck</t>
+  </si>
+  <si>
+    <t>HttpReplyIgnoreTransportFailuresCheck</t>
+  </si>
+  <si>
+    <t>ComputeNodeNameCheck</t>
+  </si>
+  <si>
+    <t>TraceNodeDetection</t>
+  </si>
+  <si>
+    <t>XMLNSCoverXMLNS</t>
+  </si>
+  <si>
+    <t>DisconnectedNode</t>
+  </si>
+  <si>
+    <t>LabelWithoutConnections</t>
+  </si>
+  <si>
+    <t>AllInputTerminalsNotConnected</t>
+  </si>
+  <si>
+    <t>LabelWithoutRouteTo</t>
+  </si>
+  <si>
+    <t>FilterNodeConnection</t>
+  </si>
+  <si>
+    <t>SoapRequestTimeOut</t>
+  </si>
+  <si>
+    <t>MessageFlowInconsistentReply</t>
+  </si>
+  <si>
+    <t>SOAPAsyncNodeFault</t>
+  </si>
+  <si>
+    <t>aggregateControlNodeTimeout</t>
+  </si>
+  <si>
+    <t>NodeNameModuleName</t>
+  </si>
+  <si>
+    <t>OneModuleMultipleNodes</t>
+  </si>
+  <si>
+    <t>NodeLevelAdditionalInstances</t>
+  </si>
+  <si>
+    <t>UnusedSubFlow</t>
+  </si>
+  <si>
+    <t>MQReplyWithoutMQInput</t>
+  </si>
+  <si>
+    <t>MQ Reply Node</t>
+  </si>
+  <si>
+    <t>The Flow contains MQ Reply node without MQ Input node.</t>
+  </si>
+  <si>
+    <t>Rule/Key</t>
   </si>
 </sst>
 </file>
@@ -3948,547 +4047,661 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="117.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="117.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>288</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>289</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>288</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>293</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>294</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>296</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>297</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>288</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>289</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>288</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>341</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>291</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>311</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" t="s">
+        <v>289</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" t="s">
+        <v>289</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="C8" t="s">
-        <v>340</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D15" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="F18" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C19" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="E19" t="s">
+        <v>297</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" t="s">
+        <v>343</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C21" t="s">
+        <v>288</v>
+      </c>
+      <c r="D21" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" t="s">
+        <v>339</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="C22" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" t="s">
+        <v>342</v>
+      </c>
+      <c r="E22" t="s">
+        <v>345</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C23" t="s">
+        <v>296</v>
+      </c>
+      <c r="D23" t="s">
+        <v>347</v>
+      </c>
+      <c r="E23" t="s">
+        <v>339</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C24" t="s">
+        <v>288</v>
+      </c>
+      <c r="D24" t="s">
+        <v>343</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C25" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" t="s">
+        <v>339</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="C26" t="s">
         <v>311</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D26" t="s">
+        <v>346</v>
+      </c>
+      <c r="E26" t="s">
         <v>289</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="F26" s="9" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C27" t="s">
+        <v>296</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E27" t="s">
+        <v>339</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C28" t="s">
+        <v>296</v>
+      </c>
+      <c r="D28" t="s">
+        <v>350</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D29" t="s">
+        <v>342</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="F29" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C30" t="s">
         <v>288</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D30" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="E30" t="s">
         <v>289</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="F30" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="C31" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B13" s="5" t="s">
+      <c r="D31" t="s">
+        <v>346</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C32" t="s">
         <v>288</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="D32" t="s">
         <v>342</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>336</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="B18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="D18" t="s">
-        <v>297</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="B19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C19" t="s">
-        <v>343</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="B20" t="s">
-        <v>288</v>
-      </c>
-      <c r="C20" t="s">
-        <v>342</v>
-      </c>
-      <c r="D20" t="s">
-        <v>339</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="B21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C21" t="s">
-        <v>342</v>
-      </c>
-      <c r="D21" t="s">
-        <v>345</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="B22" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" t="s">
-        <v>347</v>
-      </c>
-      <c r="D22" t="s">
-        <v>339</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>331</v>
-      </c>
-      <c r="B23" t="s">
-        <v>288</v>
-      </c>
-      <c r="C23" t="s">
-        <v>343</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="B24" t="s">
-        <v>296</v>
-      </c>
-      <c r="C24" t="s">
-        <v>342</v>
-      </c>
-      <c r="D24" t="s">
-        <v>339</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="B25" t="s">
-        <v>311</v>
-      </c>
-      <c r="C25" t="s">
-        <v>346</v>
-      </c>
-      <c r="D25" t="s">
-        <v>289</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="B26" t="s">
-        <v>296</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="D26" t="s">
-        <v>339</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="B27" t="s">
-        <v>296</v>
-      </c>
-      <c r="C27" t="s">
-        <v>350</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="B28" t="s">
-        <v>288</v>
-      </c>
-      <c r="C28" t="s">
-        <v>342</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="B29" t="s">
-        <v>288</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="D29" t="s">
-        <v>289</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="B30" t="s">
-        <v>288</v>
-      </c>
-      <c r="C30" t="s">
-        <v>346</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="B31" t="s">
-        <v>288</v>
-      </c>
-      <c r="C31" t="s">
-        <v>342</v>
-      </c>
-      <c r="D31" s="9" t="s">
+      <c r="E32" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>359</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finalized message map parser implementation and rules
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="400">
   <si>
     <t>severity</t>
   </si>
@@ -1213,6 +1213,27 @@
   </si>
   <si>
     <t>Rule/Key</t>
+  </si>
+  <si>
+    <t>mappingNodePropertiesMissing</t>
+  </si>
+  <si>
+    <t>todoFoundInMapping</t>
+  </si>
+  <si>
+    <t>Message Map</t>
+  </si>
+  <si>
+    <t>MINOE</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>Properties mapping missing in the message map.</t>
+  </si>
+  <si>
+    <t>TODO was block found in the message map.</t>
   </si>
 </sst>
 </file>
@@ -4047,10 +4068,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4705,6 +4726,46 @@
         <v>359</v>
       </c>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C33" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" t="s">
+        <v>341</v>
+      </c>
+      <c r="E33" t="s">
+        <v>339</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C34" t="s">
+        <v>396</v>
+      </c>
+      <c r="D34" t="s">
+        <v>397</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updating the rule-sheet and the rule definitions.
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="416">
   <si>
     <t>severity</t>
   </si>
@@ -1224,9 +1224,6 @@
     <t>Message Map</t>
   </si>
   <si>
-    <t>MINOE</t>
-  </si>
-  <si>
     <t>10 min</t>
   </si>
   <si>
@@ -1234,6 +1231,58 @@
   </si>
   <si>
     <t>TODO was block found in the message map.</t>
+  </si>
+  <si>
+    <t>queueNamingConvention</t>
+  </si>
+  <si>
+    <t>MQ Nodes</t>
+  </si>
+  <si>
+    <t>InconsistentRouteNode</t>
+  </si>
+  <si>
+    <t>DeprecatedNodeCheck</t>
+  </si>
+  <si>
+    <t>DSNWithoutDBCall</t>
+  </si>
+  <si>
+    <t>MavenProjectNamingConventions</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Compute Node</t>
+  </si>
+  <si>
+    <t>Check Node</t>
+  </si>
+  <si>
+    <t>Route Node</t>
+  </si>
+  <si>
+    <t>Usage of deprecated nodes in the message flow is discouraged.</t>
+  </si>
+  <si>
+    <t>Data Source should not be specified if compute node is not interacting with Database.</t>
+  </si>
+  <si>
+    <t>The maven project artifacts and modules should follow Naming conventions.</t>
+  </si>
+  <si>
+    <t>All the terminals specified in the filter table should be connected, otherwise it may cause abnormal termination and message might be lost.</t>
+  </si>
+  <si>
+    <t>MQ nodes should access alias queues. The naming convetion for alias queues is '^[A-Za-z0-9_]+\\.[A-Za-z0-9_]+\\.[A-Za-z0-9_]+\\.(AI|AO)$'.</t>
+  </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>Correctness,
+Performance</t>
   </si>
 </sst>
 </file>
@@ -4068,10 +4117,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4743,7 +4792,7 @@
         <v>339</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4754,16 +4803,116 @@
         <v>395</v>
       </c>
       <c r="C34" t="s">
+        <v>311</v>
+      </c>
+      <c r="D34" t="s">
         <v>396</v>
-      </c>
-      <c r="D34" t="s">
-        <v>397</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>339</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
         <v>399</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C35" t="s">
+        <v>311</v>
+      </c>
+      <c r="D35" t="s">
+        <v>341</v>
+      </c>
+      <c r="E35" t="s">
+        <v>289</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C36" t="s">
+        <v>296</v>
+      </c>
+      <c r="D36" t="s">
+        <v>347</v>
+      </c>
+      <c r="E36" t="s">
+        <v>339</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="C37" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" t="s">
+        <v>346</v>
+      </c>
+      <c r="E37" t="s">
+        <v>414</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="C38" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" t="s">
+        <v>396</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C39" t="s">
+        <v>311</v>
+      </c>
+      <c r="D39" t="s">
+        <v>342</v>
+      </c>
+      <c r="E39" t="s">
+        <v>289</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>